<commit_message>
Added Download CSV button to the print page
</commit_message>
<xml_diff>
--- a/Epi.Web/Content/Text/EmailList.xlsx
+++ b/Epi.Web/Content/Text/EmailList.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vwm5\Desktop\Epi-Info-Web-Survey\Epi.Web\Content\Text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vwm5\source\repos\Epi-Info\Epi-Info-Web-Survey\Epi.Web\Content\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11250" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
-  <si>
-    <t>Emai Address</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">ResponseId </t>
   </si>
@@ -51,9 +51,6 @@
     <t>Sender</t>
   </si>
   <si>
-    <t>sax5@cdc.gov</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -100,6 +97,15 @@
   </si>
   <si>
     <t>Reminder email</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Send Email</t>
+  </si>
+  <si>
+    <t>epiinfo@cdc.gov</t>
   </si>
 </sst>
 </file>
@@ -529,83 +535,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="52.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="23.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24" style="2" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="23.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3">
+      <c r="K3">
         <v>33</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -616,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,44 +647,44 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>